<commit_message>
자바 This, Final, Static, Getter, Setter 수업
</commit_message>
<xml_diff>
--- a/스터디 기록.xlsx
+++ b/스터디 기록.xlsx
@@ -19,15 +19,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="31">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="31">
   <x:si>
     <x:t>술 먹은사람(기본+술+음료수4개)</x:t>
   </x:si>
   <x:si>
-    <x:t>총 참여 횟수</x:t>
+    <x:t>김아영</x:t>
   </x:si>
   <x:si>
-    <x:t>술 먹은 사람</x:t>
+    <x:t>소주</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기본</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정근승</x:t>
+  </x:si>
+  <x:si>
+    <x:t>남현우</x:t>
+  </x:si>
+  <x:si>
+    <x:t>뼈추가</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이름</x:t>
+  </x:si>
+  <x:si>
+    <x:t>박규태</x:t>
+  </x:si>
+  <x:si>
+    <x:t>김소원</x:t>
+  </x:si>
+  <x:si>
+    <x:t>요일</x:t>
+  </x:si>
+  <x:si>
+    <x:t>박경민</x:t>
+  </x:si>
+  <x:si>
+    <x:t>날짜</x:t>
+  </x:si>
+  <x:si>
+    <x:t>김승환</x:t>
+  </x:si>
+  <x:si>
+    <x:t>볶음밥</x:t>
+  </x:si>
+  <x:si>
+    <x:t>조민정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>맥주</x:t>
+  </x:si>
+  <x:si>
+    <x:t>감자탕</x:t>
+  </x:si>
+  <x:si>
+    <x:t>총인원</x:t>
+  </x:si>
+  <x:si>
+    <x:t>현준수</x:t>
+  </x:si>
+  <x:si>
+    <x:t>음료수</x:t>
+  </x:si>
+  <x:si>
+    <x:t>o</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이정은</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이제섭</x:t>
   </x:si>
   <x:si>
     <x:t>술 안먹은사람(기본+음료수)</x:t>
@@ -45,73 +108,10 @@
     <x:t>술 안먹은사람 2명</x:t>
   </x:si>
   <x:si>
-    <x:t>요일</x:t>
+    <x:t>술 먹은 사람</x:t>
   </x:si>
   <x:si>
-    <x:t>박경민</x:t>
-  </x:si>
-  <x:si>
-    <x:t>김승환</x:t>
-  </x:si>
-  <x:si>
-    <x:t>소주</x:t>
-  </x:si>
-  <x:si>
-    <x:t>날짜</x:t>
-  </x:si>
-  <x:si>
-    <x:t>박규태</x:t>
-  </x:si>
-  <x:si>
-    <x:t>조민정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>맥주</x:t>
-  </x:si>
-  <x:si>
-    <x:t>감자탕</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기본</x:t>
-  </x:si>
-  <x:si>
-    <x:t>볶음밥</x:t>
-  </x:si>
-  <x:si>
-    <x:t>남현우</x:t>
-  </x:si>
-  <x:si>
-    <x:t>김소원</x:t>
-  </x:si>
-  <x:si>
-    <x:t>뼈추가</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이름</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정근승</x:t>
-  </x:si>
-  <x:si>
-    <x:t>김아영</x:t>
-  </x:si>
-  <x:si>
-    <x:t>o</x:t>
-  </x:si>
-  <x:si>
-    <x:t>현준수</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이정은</x:t>
-  </x:si>
-  <x:si>
-    <x:t>총인원</x:t>
-  </x:si>
-  <x:si>
-    <x:t>음료수</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이제섭</x:t>
+    <x:t>총 참여 횟수</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -322,16 +322,16 @@
       </x:bottom>
     </x:border>
     <x:border>
-      <x:left>
+      <x:left style="thin">
         <x:color indexed="64"/>
       </x:left>
       <x:right>
         <x:color indexed="64"/>
       </x:right>
-      <x:top style="thin">
+      <x:top>
         <x:color indexed="64"/>
       </x:top>
-      <x:bottom>
+      <x:bottom style="thin">
         <x:color indexed="64"/>
       </x:bottom>
     </x:border>
@@ -339,7 +339,7 @@
       <x:left>
         <x:color indexed="64"/>
       </x:left>
-      <x:right style="thin">
+      <x:right>
         <x:color indexed="64"/>
       </x:right>
       <x:top style="thin">
@@ -350,16 +350,16 @@
       </x:bottom>
     </x:border>
     <x:border>
-      <x:left style="thin">
+      <x:left>
         <x:color indexed="64"/>
       </x:left>
-      <x:right>
+      <x:right style="thin">
         <x:color indexed="64"/>
       </x:right>
-      <x:top>
+      <x:top style="thin">
         <x:color indexed="64"/>
       </x:top>
-      <x:bottom style="thin">
+      <x:bottom>
         <x:color indexed="64"/>
       </x:bottom>
     </x:border>
@@ -677,6 +677,58 @@
     </x:xf>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="165" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="165" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="165" fontId="6" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="165" fontId="6" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
           <x:alignment horizontal="center" vertical="center"/>
           <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
@@ -684,6 +736,32 @@
       </mc:Choice>
       <mc:Fallback>
         <x:xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
           <x:alignment horizontal="center" vertical="center"/>
         </x:xf>
       </mc:Fallback>
@@ -703,32 +781,6 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
           <x:alignment horizontal="center" vertical="center"/>
           <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
@@ -879,58 +931,6 @@
       </mc:Choice>
       <mc:Fallback>
         <x:xf numFmtId="164" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="165" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="165" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="165" fontId="6" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="165" fontId="6" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
           <x:alignment horizontal="center" vertical="center"/>
         </x:xf>
       </mc:Fallback>
@@ -1613,106 +1613,105 @@
   <x:dimension ref="A1:M35"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="A1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="E26" activeCellId="0" sqref="E26:E26"/>
+      <x:selection activeCell="L19" activeCellId="0" sqref="L19:L19"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.75"/>
   <x:cols>
     <x:col min="1" max="1" width="9.5625" style="1" bestFit="1" customWidth="1"/>
-    <x:col min="2" max="2" width="4.2734375" style="32" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="4.2734375" style="16" bestFit="1" customWidth="1"/>
     <x:col min="3" max="4" width="5.8046875" style="1" bestFit="1" customWidth="1"/>
     <x:col min="5" max="8" width="5.9921875" style="1" bestFit="1" customWidth="1"/>
     <x:col min="9" max="9" width="6.1796875" style="1" bestFit="1" customWidth="1"/>
     <x:col min="10" max="10" width="5.8046875" style="1" bestFit="1" customWidth="1"/>
     <x:col min="11" max="11" width="5.9921875" style="1" bestFit="1" customWidth="1"/>
     <x:col min="12" max="13" width="5.8046875" style="1" bestFit="1" customWidth="1"/>
-    <x:col min="14" max="16383" width="8.88671875" style="1"/>
-    <x:col min="16384" max="16384" width="8.88671875" style="1"/>
+    <x:col min="14" max="16384" width="8.88671875" style="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:13" customHeight="1">
       <x:c r="A1" s="2" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="B1" s="33"/>
-      <x:c r="C1" s="16" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="D1" s="17"/>
-      <x:c r="E1" s="17"/>
-      <x:c r="F1" s="17"/>
-      <x:c r="G1" s="17"/>
-      <x:c r="H1" s="17"/>
-      <x:c r="I1" s="17"/>
-      <x:c r="J1" s="17"/>
-      <x:c r="K1" s="17"/>
-      <x:c r="L1" s="17"/>
-      <x:c r="M1" s="18"/>
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B1" s="17"/>
+      <x:c r="C1" s="20" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D1" s="21"/>
+      <x:c r="E1" s="21"/>
+      <x:c r="F1" s="21"/>
+      <x:c r="G1" s="21"/>
+      <x:c r="H1" s="21"/>
+      <x:c r="I1" s="21"/>
+      <x:c r="J1" s="21"/>
+      <x:c r="K1" s="21"/>
+      <x:c r="L1" s="21"/>
+      <x:c r="M1" s="22"/>
     </x:row>
     <x:row r="2" spans="1:13" customHeight="1">
       <x:c r="A2" s="2">
         <x:f>COUNTA(C3:M3)</x:f>
         <x:v>11</x:v>
       </x:c>
-      <x:c r="B2" s="34"/>
-      <x:c r="C2" s="19"/>
-      <x:c r="D2" s="20"/>
-      <x:c r="E2" s="20"/>
-      <x:c r="F2" s="20"/>
-      <x:c r="G2" s="20"/>
-      <x:c r="H2" s="20"/>
-      <x:c r="I2" s="20"/>
-      <x:c r="J2" s="20"/>
-      <x:c r="K2" s="20"/>
-      <x:c r="L2" s="20"/>
-      <x:c r="M2" s="21"/>
+      <x:c r="B2" s="18"/>
+      <x:c r="C2" s="23"/>
+      <x:c r="D2" s="24"/>
+      <x:c r="E2" s="24"/>
+      <x:c r="F2" s="24"/>
+      <x:c r="G2" s="24"/>
+      <x:c r="H2" s="24"/>
+      <x:c r="I2" s="24"/>
+      <x:c r="J2" s="24"/>
+      <x:c r="K2" s="24"/>
+      <x:c r="L2" s="24"/>
+      <x:c r="M2" s="25"/>
     </x:row>
     <x:row r="3" spans="1:13">
       <x:c r="A3" s="2" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="B3" s="35" t="s">
+      <x:c r="B3" s="19" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C3" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="D3" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E3" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="F3" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="G3" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="H3" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="I3" s="2" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="C3" s="2" t="s">
+      <x:c r="J3" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="K3" s="2" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="D3" s="2" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="E3" s="2" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="F3" s="2" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="G3" s="2" t="s">
+      <x:c r="L3" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="M3" s="2" t="s">
         <x:v>19</x:v>
-      </x:c>
-      <x:c r="H3" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="I3" s="2" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="J3" s="2" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="K3" s="2" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="L3" s="2" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="M3" s="2" t="s">
-        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:13">
       <x:c r="A4" s="3">
         <x:v>45474</x:v>
       </x:c>
-      <x:c r="B4" s="35">
+      <x:c r="B4" s="19">
         <x:f>A4</x:f>
         <x:v>45474</x:v>
       </x:c>
@@ -1733,19 +1732,23 @@
         <x:f>A4+1</x:f>
         <x:v>45475</x:v>
       </x:c>
-      <x:c r="B5" s="35">
+      <x:c r="B5" s="19">
         <x:f t="shared" ref="B5:B34" si="0">A5</x:f>
         <x:v>45475</x:v>
       </x:c>
       <x:c r="C5" s="6"/>
       <x:c r="D5" s="6"/>
       <x:c r="E5" s="6"/>
-      <x:c r="F5" s="6"/>
+      <x:c r="F5" s="5" t="s">
+        <x:v>21</x:v>
+      </x:c>
       <x:c r="G5" s="6"/>
       <x:c r="H5" s="6"/>
       <x:c r="I5" s="6"/>
       <x:c r="J5" s="6"/>
-      <x:c r="K5" s="6"/>
+      <x:c r="K5" s="5" t="s">
+        <x:v>21</x:v>
+      </x:c>
       <x:c r="L5" s="6"/>
       <x:c r="M5" s="6"/>
     </x:row>
@@ -1754,7 +1757,7 @@
         <x:f t="shared" ref="A6:A34" si="1">A5+1</x:f>
         <x:v>45476</x:v>
       </x:c>
-      <x:c r="B6" s="35">
+      <x:c r="B6" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45476</x:v>
       </x:c>
@@ -1775,28 +1778,36 @@
         <x:f t="shared" si="1"/>
         <x:v>45477</x:v>
       </x:c>
-      <x:c r="B7" s="35">
+      <x:c r="B7" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45477</x:v>
       </x:c>
       <x:c r="C7" s="6"/>
       <x:c r="D7" s="6"/>
-      <x:c r="E7" s="6"/>
-      <x:c r="F7" s="6"/>
+      <x:c r="E7" s="5" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="F7" s="5" t="s">
+        <x:v>21</x:v>
+      </x:c>
       <x:c r="G7" s="6"/>
       <x:c r="H7" s="6"/>
       <x:c r="I7" s="6"/>
       <x:c r="J7" s="6"/>
       <x:c r="K7" s="6"/>
-      <x:c r="L7" s="6"/>
-      <x:c r="M7" s="6"/>
+      <x:c r="L7" s="5" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="M7" s="5" t="s">
+        <x:v>21</x:v>
+      </x:c>
     </x:row>
     <x:row r="8" spans="1:13">
       <x:c r="A8" s="3">
         <x:f t="shared" si="1"/>
         <x:v>45478</x:v>
       </x:c>
-      <x:c r="B8" s="35">
+      <x:c r="B8" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45478</x:v>
       </x:c>
@@ -1817,16 +1828,20 @@
         <x:f t="shared" si="1"/>
         <x:v>45479</x:v>
       </x:c>
-      <x:c r="B9" s="35">
+      <x:c r="B9" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45479</x:v>
       </x:c>
-      <x:c r="C9" s="6"/>
+      <x:c r="C9" s="5" t="s">
+        <x:v>21</x:v>
+      </x:c>
       <x:c r="D9" s="6"/>
       <x:c r="E9" s="6"/>
       <x:c r="F9" s="6"/>
       <x:c r="G9" s="6"/>
-      <x:c r="H9" s="6"/>
+      <x:c r="H9" s="5" t="s">
+        <x:v>21</x:v>
+      </x:c>
       <x:c r="I9" s="6"/>
       <x:c r="J9" s="6"/>
       <x:c r="K9" s="6"/>
@@ -1838,28 +1853,40 @@
         <x:f t="shared" si="1"/>
         <x:v>45480</x:v>
       </x:c>
-      <x:c r="B10" s="35">
+      <x:c r="B10" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45480</x:v>
       </x:c>
       <x:c r="C10" s="6"/>
       <x:c r="D10" s="6"/>
-      <x:c r="E10" s="6"/>
-      <x:c r="F10" s="6"/>
+      <x:c r="E10" s="5" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="F10" s="5" t="s">
+        <x:v>21</x:v>
+      </x:c>
       <x:c r="G10" s="6"/>
       <x:c r="H10" s="6"/>
       <x:c r="I10" s="6"/>
-      <x:c r="J10" s="6"/>
-      <x:c r="K10" s="6"/>
-      <x:c r="L10" s="6"/>
-      <x:c r="M10" s="6"/>
+      <x:c r="J10" s="5" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="K10" s="5" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L10" s="5" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="M10" s="5" t="s">
+        <x:v>21</x:v>
+      </x:c>
     </x:row>
     <x:row r="11" spans="1:13">
       <x:c r="A11" s="3">
         <x:f t="shared" si="1"/>
         <x:v>45481</x:v>
       </x:c>
-      <x:c r="B11" s="35">
+      <x:c r="B11" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45481</x:v>
       </x:c>
@@ -1880,7 +1907,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45482</x:v>
       </x:c>
-      <x:c r="B12" s="35">
+      <x:c r="B12" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45482</x:v>
       </x:c>
@@ -1901,7 +1928,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45483</x:v>
       </x:c>
-      <x:c r="B13" s="35">
+      <x:c r="B13" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45483</x:v>
       </x:c>
@@ -1922,7 +1949,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45484</x:v>
       </x:c>
-      <x:c r="B14" s="35">
+      <x:c r="B14" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45484</x:v>
       </x:c>
@@ -1943,7 +1970,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45485</x:v>
       </x:c>
-      <x:c r="B15" s="35">
+      <x:c r="B15" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45485</x:v>
       </x:c>
@@ -1964,7 +1991,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45486</x:v>
       </x:c>
-      <x:c r="B16" s="35">
+      <x:c r="B16" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45486</x:v>
       </x:c>
@@ -1985,7 +2012,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45487</x:v>
       </x:c>
-      <x:c r="B17" s="35">
+      <x:c r="B17" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45487</x:v>
       </x:c>
@@ -2006,7 +2033,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45488</x:v>
       </x:c>
-      <x:c r="B18" s="35">
+      <x:c r="B18" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45488</x:v>
       </x:c>
@@ -2027,7 +2054,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45489</x:v>
       </x:c>
-      <x:c r="B19" s="35">
+      <x:c r="B19" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45489</x:v>
       </x:c>
@@ -2048,7 +2075,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45490</x:v>
       </x:c>
-      <x:c r="B20" s="35">
+      <x:c r="B20" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45490</x:v>
       </x:c>
@@ -2069,7 +2096,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45491</x:v>
       </x:c>
-      <x:c r="B21" s="35">
+      <x:c r="B21" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45491</x:v>
       </x:c>
@@ -2090,7 +2117,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45492</x:v>
       </x:c>
-      <x:c r="B22" s="35">
+      <x:c r="B22" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45492</x:v>
       </x:c>
@@ -2111,7 +2138,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45493</x:v>
       </x:c>
-      <x:c r="B23" s="35">
+      <x:c r="B23" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45493</x:v>
       </x:c>
@@ -2132,7 +2159,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45494</x:v>
       </x:c>
-      <x:c r="B24" s="35">
+      <x:c r="B24" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45494</x:v>
       </x:c>
@@ -2153,7 +2180,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45495</x:v>
       </x:c>
-      <x:c r="B25" s="35">
+      <x:c r="B25" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45495</x:v>
       </x:c>
@@ -2174,7 +2201,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45496</x:v>
       </x:c>
-      <x:c r="B26" s="35">
+      <x:c r="B26" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45496</x:v>
       </x:c>
@@ -2195,7 +2222,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45497</x:v>
       </x:c>
-      <x:c r="B27" s="35">
+      <x:c r="B27" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45497</x:v>
       </x:c>
@@ -2216,7 +2243,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45498</x:v>
       </x:c>
-      <x:c r="B28" s="35">
+      <x:c r="B28" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45498</x:v>
       </x:c>
@@ -2237,7 +2264,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45499</x:v>
       </x:c>
-      <x:c r="B29" s="35">
+      <x:c r="B29" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45499</x:v>
       </x:c>
@@ -2258,7 +2285,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45500</x:v>
       </x:c>
-      <x:c r="B30" s="35">
+      <x:c r="B30" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45500</x:v>
       </x:c>
@@ -2279,7 +2306,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45501</x:v>
       </x:c>
-      <x:c r="B31" s="35">
+      <x:c r="B31" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45501</x:v>
       </x:c>
@@ -2300,7 +2327,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45502</x:v>
       </x:c>
-      <x:c r="B32" s="35">
+      <x:c r="B32" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45502</x:v>
       </x:c>
@@ -2321,7 +2348,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45503</x:v>
       </x:c>
-      <x:c r="B33" s="35">
+      <x:c r="B33" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45503</x:v>
       </x:c>
@@ -2342,7 +2369,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45504</x:v>
       </x:c>
-      <x:c r="B34" s="35">
+      <x:c r="B34" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45504</x:v>
       </x:c>
@@ -2360,12 +2387,12 @@
     </x:row>
     <x:row r="35" spans="1:13">
       <x:c r="A35" s="4" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="B35" s="35"/>
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B35" s="19"/>
       <x:c r="C35" s="2">
         <x:f>COUNTA(C4:C34)</x:f>
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="D35" s="2">
         <x:f t="shared" ref="D35:M35" si="2">COUNTA(D4:D34)</x:f>
@@ -2373,11 +2400,11 @@
       </x:c>
       <x:c r="E35" s="2">
         <x:f t="shared" si="2"/>
-        <x:v>0</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="F35" s="2">
         <x:f t="shared" si="2"/>
-        <x:v>0</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="G35" s="2">
         <x:f t="shared" si="2"/>
@@ -2385,7 +2412,7 @@
       </x:c>
       <x:c r="H35" s="2">
         <x:f t="shared" si="2"/>
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="I35" s="2">
         <x:f t="shared" si="2"/>
@@ -2393,19 +2420,19 @@
       </x:c>
       <x:c r="J35" s="2">
         <x:f t="shared" si="2"/>
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="K35" s="2">
         <x:f t="shared" si="2"/>
-        <x:v>0</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="L35" s="2">
         <x:f t="shared" si="2"/>
-        <x:v>0</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="M35" s="2">
         <x:f t="shared" si="2"/>
-        <x:v>0</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -2439,115 +2466,114 @@
   <x:dimension ref="A1:M35"/>
   <x:sheetViews>
     <x:sheetView topLeftCell="A1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="H16" activeCellId="0" sqref="H16:H16"/>
+      <x:selection activeCell="F15" activeCellId="0" sqref="F15:F15"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.75"/>
   <x:cols>
     <x:col min="1" max="1" width="9.5625" style="1" bestFit="1" customWidth="1"/>
-    <x:col min="2" max="2" width="4.2734375" style="32" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="4.2734375" style="16" bestFit="1" customWidth="1"/>
     <x:col min="3" max="4" width="5.8046875" style="1" bestFit="1" customWidth="1"/>
     <x:col min="5" max="8" width="5.9921875" style="1" bestFit="1" customWidth="1"/>
     <x:col min="9" max="9" width="6.1796875" style="1" bestFit="1" customWidth="1"/>
     <x:col min="10" max="10" width="5.8046875" style="1" bestFit="1" customWidth="1"/>
     <x:col min="11" max="11" width="5.9921875" style="1" bestFit="1" customWidth="1"/>
     <x:col min="12" max="13" width="5.8046875" style="1" bestFit="1" customWidth="1"/>
-    <x:col min="14" max="16383" width="8.88671875" style="1"/>
-    <x:col min="16384" max="16384" width="8.88671875" style="1"/>
+    <x:col min="14" max="16384" width="8.88671875" style="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:13" customHeight="1">
       <x:c r="A1" s="2" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="B1" s="33"/>
-      <x:c r="C1" s="16" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="D1" s="17"/>
-      <x:c r="E1" s="17"/>
-      <x:c r="F1" s="17"/>
-      <x:c r="G1" s="17"/>
-      <x:c r="H1" s="17"/>
-      <x:c r="I1" s="17"/>
-      <x:c r="J1" s="17"/>
-      <x:c r="K1" s="17"/>
-      <x:c r="L1" s="17"/>
-      <x:c r="M1" s="18"/>
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B1" s="17"/>
+      <x:c r="C1" s="20" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D1" s="21"/>
+      <x:c r="E1" s="21"/>
+      <x:c r="F1" s="21"/>
+      <x:c r="G1" s="21"/>
+      <x:c r="H1" s="21"/>
+      <x:c r="I1" s="21"/>
+      <x:c r="J1" s="21"/>
+      <x:c r="K1" s="21"/>
+      <x:c r="L1" s="21"/>
+      <x:c r="M1" s="22"/>
     </x:row>
     <x:row r="2" spans="1:13" customHeight="1">
       <x:c r="A2" s="2">
         <x:f>COUNTA(C3:M3)</x:f>
         <x:v>11</x:v>
       </x:c>
-      <x:c r="B2" s="34"/>
-      <x:c r="C2" s="19"/>
-      <x:c r="D2" s="20"/>
-      <x:c r="E2" s="20"/>
-      <x:c r="F2" s="20"/>
-      <x:c r="G2" s="20"/>
-      <x:c r="H2" s="20"/>
-      <x:c r="I2" s="20"/>
-      <x:c r="J2" s="20"/>
-      <x:c r="K2" s="20"/>
-      <x:c r="L2" s="20"/>
-      <x:c r="M2" s="21"/>
+      <x:c r="B2" s="18"/>
+      <x:c r="C2" s="23"/>
+      <x:c r="D2" s="24"/>
+      <x:c r="E2" s="24"/>
+      <x:c r="F2" s="24"/>
+      <x:c r="G2" s="24"/>
+      <x:c r="H2" s="24"/>
+      <x:c r="I2" s="24"/>
+      <x:c r="J2" s="24"/>
+      <x:c r="K2" s="24"/>
+      <x:c r="L2" s="24"/>
+      <x:c r="M2" s="25"/>
     </x:row>
     <x:row r="3" spans="1:13">
       <x:c r="A3" s="2" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="B3" s="35" t="s">
+      <x:c r="B3" s="19" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C3" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="D3" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E3" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="F3" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="G3" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="H3" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="I3" s="2" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="C3" s="2" t="s">
+      <x:c r="J3" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="K3" s="2" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="D3" s="2" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="E3" s="2" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="F3" s="2" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="G3" s="2" t="s">
+      <x:c r="L3" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="M3" s="2" t="s">
         <x:v>19</x:v>
-      </x:c>
-      <x:c r="H3" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="I3" s="2" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="J3" s="2" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="K3" s="2" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="L3" s="2" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="M3" s="2" t="s">
-        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:13">
       <x:c r="A4" s="3">
         <x:v>45443</x:v>
       </x:c>
-      <x:c r="B4" s="35">
+      <x:c r="B4" s="19">
         <x:f>A4</x:f>
         <x:v>45443</x:v>
       </x:c>
       <x:c r="C4" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D4" s="6"/>
       <x:c r="E4" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="F4" s="6"/>
       <x:c r="G4" s="6"/>
@@ -2563,19 +2589,19 @@
         <x:f>A4+1</x:f>
         <x:v>45444</x:v>
       </x:c>
-      <x:c r="B5" s="35">
+      <x:c r="B5" s="19">
         <x:f t="shared" ref="B5:B34" si="0">A5</x:f>
         <x:v>45444</x:v>
       </x:c>
       <x:c r="C5" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D5" s="6"/>
       <x:c r="E5" s="6"/>
       <x:c r="F5" s="6"/>
       <x:c r="G5" s="6"/>
       <x:c r="H5" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="I5" s="6"/>
       <x:c r="J5" s="6"/>
@@ -2588,14 +2614,14 @@
         <x:f t="shared" ref="A6:A34" si="1">A5+1</x:f>
         <x:v>45445</x:v>
       </x:c>
-      <x:c r="B6" s="35">
+      <x:c r="B6" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45445</x:v>
       </x:c>
       <x:c r="C6" s="6"/>
       <x:c r="D6" s="6"/>
       <x:c r="E6" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="F6" s="6"/>
       <x:c r="G6" s="6"/>
@@ -2611,7 +2637,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45446</x:v>
       </x:c>
-      <x:c r="B7" s="35">
+      <x:c r="B7" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45446</x:v>
       </x:c>
@@ -2632,24 +2658,24 @@
         <x:f t="shared" si="1"/>
         <x:v>45447</x:v>
       </x:c>
-      <x:c r="B8" s="35">
+      <x:c r="B8" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45447</x:v>
       </x:c>
       <x:c r="C8" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D8" s="6"/>
       <x:c r="E8" s="6"/>
       <x:c r="F8" s="6"/>
       <x:c r="G8" s="6"/>
       <x:c r="H8" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="I8" s="6"/>
       <x:c r="J8" s="6"/>
       <x:c r="K8" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L8" s="6"/>
       <x:c r="M8" s="6"/>
@@ -2659,7 +2685,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45448</x:v>
       </x:c>
-      <x:c r="B9" s="35">
+      <x:c r="B9" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45448</x:v>
       </x:c>
@@ -2680,32 +2706,32 @@
         <x:f t="shared" si="1"/>
         <x:v>45449</x:v>
       </x:c>
-      <x:c r="B10" s="35">
+      <x:c r="B10" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45449</x:v>
       </x:c>
       <x:c r="C10" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D10" s="6"/>
       <x:c r="E10" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="F10" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="G10" s="6"/>
       <x:c r="H10" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="I10" s="6"/>
       <x:c r="J10" s="6"/>
       <x:c r="K10" s="6"/>
       <x:c r="L10" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="M10" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:13">
@@ -2713,19 +2739,19 @@
         <x:f t="shared" si="1"/>
         <x:v>45450</x:v>
       </x:c>
-      <x:c r="B11" s="35">
+      <x:c r="B11" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45450</x:v>
       </x:c>
       <x:c r="C11" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D11" s="6"/>
       <x:c r="E11" s="6"/>
       <x:c r="F11" s="6"/>
       <x:c r="G11" s="6"/>
       <x:c r="H11" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="I11" s="6"/>
       <x:c r="J11" s="6"/>
@@ -2738,7 +2764,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45451</x:v>
       </x:c>
-      <x:c r="B12" s="35">
+      <x:c r="B12" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45451</x:v>
       </x:c>
@@ -2747,18 +2773,18 @@
       <x:c r="E12" s="6"/>
       <x:c r="F12" s="6"/>
       <x:c r="G12" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="H12" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="I12" s="6"/>
       <x:c r="J12" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="K12" s="6"/>
       <x:c r="L12" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="M12" s="6"/>
     </x:row>
@@ -2767,34 +2793,34 @@
         <x:f t="shared" si="1"/>
         <x:v>45452</x:v>
       </x:c>
-      <x:c r="B13" s="35">
+      <x:c r="B13" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45452</x:v>
       </x:c>
       <x:c r="C13" s="6"/>
       <x:c r="D13" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E13" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="F13" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="G13" s="6"/>
       <x:c r="H13" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="I13" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="J13" s="6"/>
       <x:c r="K13" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L13" s="6"/>
       <x:c r="M13" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:13">
@@ -2802,7 +2828,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45453</x:v>
       </x:c>
-      <x:c r="B14" s="35">
+      <x:c r="B14" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45453</x:v>
       </x:c>
@@ -2810,7 +2836,7 @@
       <x:c r="D14" s="6"/>
       <x:c r="E14" s="6"/>
       <x:c r="F14" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="G14" s="6"/>
       <x:c r="H14" s="6"/>
@@ -2825,36 +2851,36 @@
         <x:f t="shared" si="1"/>
         <x:v>45454</x:v>
       </x:c>
-      <x:c r="B15" s="35">
+      <x:c r="B15" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45454</x:v>
       </x:c>
       <x:c r="C15" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D15" s="6"/>
       <x:c r="E15" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="F15" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="G15" s="6"/>
       <x:c r="H15" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="I15" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="J15" s="6"/>
       <x:c r="K15" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L15" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="M15" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:13">
@@ -2862,31 +2888,31 @@
         <x:f t="shared" si="1"/>
         <x:v>45455</x:v>
       </x:c>
-      <x:c r="B16" s="35">
+      <x:c r="B16" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45455</x:v>
       </x:c>
       <x:c r="C16" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D16" s="6"/>
       <x:c r="E16" s="6"/>
       <x:c r="F16" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="G16" s="6"/>
       <x:c r="H16" s="6"/>
       <x:c r="I16" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="J16" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="K16" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L16" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="M16" s="6"/>
     </x:row>
@@ -2895,7 +2921,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45456</x:v>
       </x:c>
-      <x:c r="B17" s="35">
+      <x:c r="B17" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45456</x:v>
       </x:c>
@@ -2916,7 +2942,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45457</x:v>
       </x:c>
-      <x:c r="B18" s="35">
+      <x:c r="B18" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45457</x:v>
       </x:c>
@@ -2937,26 +2963,26 @@
         <x:f t="shared" si="1"/>
         <x:v>45458</x:v>
       </x:c>
-      <x:c r="B19" s="35">
+      <x:c r="B19" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45458</x:v>
       </x:c>
       <x:c r="C19" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D19" s="6"/>
       <x:c r="E19" s="6"/>
       <x:c r="F19" s="6"/>
       <x:c r="G19" s="6"/>
       <x:c r="H19" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="I19" s="6"/>
       <x:c r="J19" s="6"/>
       <x:c r="K19" s="6"/>
       <x:c r="L19" s="6"/>
       <x:c r="M19" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:13">
@@ -2964,30 +2990,30 @@
         <x:f t="shared" si="1"/>
         <x:v>45459</x:v>
       </x:c>
-      <x:c r="B20" s="35">
+      <x:c r="B20" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45459</x:v>
       </x:c>
       <x:c r="C20" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D20" s="6"/>
       <x:c r="E20" s="6"/>
       <x:c r="F20" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="G20" s="6"/>
       <x:c r="H20" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="I20" s="6"/>
       <x:c r="J20" s="6"/>
       <x:c r="K20" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L20" s="6"/>
       <x:c r="M20" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:13">
@@ -2995,12 +3021,12 @@
         <x:f t="shared" si="1"/>
         <x:v>45460</x:v>
       </x:c>
-      <x:c r="B21" s="35">
+      <x:c r="B21" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45460</x:v>
       </x:c>
       <x:c r="C21" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D21" s="6"/>
       <x:c r="E21" s="6"/>
@@ -3009,7 +3035,7 @@
       <x:c r="H21" s="6"/>
       <x:c r="I21" s="6"/>
       <x:c r="J21" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="K21" s="6"/>
       <x:c r="L21" s="6"/>
@@ -3020,19 +3046,19 @@
         <x:f t="shared" si="1"/>
         <x:v>45461</x:v>
       </x:c>
-      <x:c r="B22" s="35">
+      <x:c r="B22" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45461</x:v>
       </x:c>
       <x:c r="C22" s="6"/>
       <x:c r="D22" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E22" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="F22" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="G22" s="6"/>
       <x:c r="H22" s="6"/>
@@ -3047,7 +3073,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45462</x:v>
       </x:c>
-      <x:c r="B23" s="35">
+      <x:c r="B23" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45462</x:v>
       </x:c>
@@ -3055,14 +3081,14 @@
       <x:c r="D23" s="6"/>
       <x:c r="E23" s="6"/>
       <x:c r="F23" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="G23" s="6"/>
       <x:c r="H23" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="I23" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="J23" s="6"/>
       <x:c r="K23" s="6"/>
@@ -3074,13 +3100,13 @@
         <x:f t="shared" si="1"/>
         <x:v>45463</x:v>
       </x:c>
-      <x:c r="B24" s="35">
+      <x:c r="B24" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45463</x:v>
       </x:c>
       <x:c r="C24" s="6"/>
       <x:c r="D24" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E24" s="6"/>
       <x:c r="F24" s="6"/>
@@ -3090,7 +3116,7 @@
       <x:c r="J24" s="6"/>
       <x:c r="K24" s="6"/>
       <x:c r="L24" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="M24" s="6"/>
     </x:row>
@@ -3099,7 +3125,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45464</x:v>
       </x:c>
-      <x:c r="B25" s="35">
+      <x:c r="B25" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45464</x:v>
       </x:c>
@@ -3107,7 +3133,7 @@
       <x:c r="D25" s="6"/>
       <x:c r="E25" s="6"/>
       <x:c r="F25" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="G25" s="6"/>
       <x:c r="H25" s="6"/>
@@ -3122,7 +3148,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45465</x:v>
       </x:c>
-      <x:c r="B26" s="35">
+      <x:c r="B26" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45465</x:v>
       </x:c>
@@ -3132,14 +3158,14 @@
       <x:c r="F26" s="6"/>
       <x:c r="G26" s="6"/>
       <x:c r="H26" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="I26" s="6"/>
       <x:c r="J26" s="6"/>
       <x:c r="K26" s="6"/>
       <x:c r="L26" s="6"/>
       <x:c r="M26" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:13">
@@ -3147,14 +3173,14 @@
         <x:f t="shared" si="1"/>
         <x:v>45466</x:v>
       </x:c>
-      <x:c r="B27" s="35">
+      <x:c r="B27" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45466</x:v>
       </x:c>
       <x:c r="C27" s="6"/>
       <x:c r="D27" s="6"/>
       <x:c r="E27" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="F27" s="6"/>
       <x:c r="G27" s="6"/>
@@ -3162,11 +3188,11 @@
       <x:c r="I27" s="6"/>
       <x:c r="J27" s="6"/>
       <x:c r="K27" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L27" s="6"/>
       <x:c r="M27" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:13">
@@ -3174,7 +3200,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45467</x:v>
       </x:c>
-      <x:c r="B28" s="35">
+      <x:c r="B28" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45467</x:v>
       </x:c>
@@ -3182,11 +3208,11 @@
       <x:c r="D28" s="6"/>
       <x:c r="E28" s="6"/>
       <x:c r="F28" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="G28" s="6"/>
       <x:c r="H28" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="I28" s="6"/>
       <x:c r="J28" s="6"/>
@@ -3199,26 +3225,26 @@
         <x:f t="shared" si="1"/>
         <x:v>45468</x:v>
       </x:c>
-      <x:c r="B29" s="35">
+      <x:c r="B29" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45468</x:v>
       </x:c>
       <x:c r="C29" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D29" s="6"/>
       <x:c r="E29" s="6"/>
       <x:c r="F29" s="6"/>
       <x:c r="G29" s="6"/>
       <x:c r="H29" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="I29" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="J29" s="6"/>
       <x:c r="K29" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L29" s="6"/>
       <x:c r="M29" s="6"/>
@@ -3228,13 +3254,13 @@
         <x:f t="shared" si="1"/>
         <x:v>45469</x:v>
       </x:c>
-      <x:c r="B30" s="35">
+      <x:c r="B30" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45469</x:v>
       </x:c>
       <x:c r="C30" s="6"/>
       <x:c r="D30" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E30" s="6"/>
       <x:c r="F30" s="6"/>
@@ -3243,11 +3269,11 @@
       <x:c r="I30" s="6"/>
       <x:c r="J30" s="6"/>
       <x:c r="K30" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L30" s="6"/>
       <x:c r="M30" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:13">
@@ -3255,30 +3281,30 @@
         <x:f t="shared" si="1"/>
         <x:v>45470</x:v>
       </x:c>
-      <x:c r="B31" s="35">
+      <x:c r="B31" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45470</x:v>
       </x:c>
       <x:c r="C31" s="6"/>
       <x:c r="D31" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E31" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="F31" s="6"/>
       <x:c r="G31" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="H31" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="I31" s="6"/>
       <x:c r="J31" s="6"/>
       <x:c r="K31" s="6"/>
       <x:c r="L31" s="6"/>
       <x:c r="M31" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:13">
@@ -3286,7 +3312,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45471</x:v>
       </x:c>
-      <x:c r="B32" s="35">
+      <x:c r="B32" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45471</x:v>
       </x:c>
@@ -3307,7 +3333,7 @@
         <x:f t="shared" si="1"/>
         <x:v>45472</x:v>
       </x:c>
-      <x:c r="B33" s="35">
+      <x:c r="B33" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45472</x:v>
       </x:c>
@@ -3328,37 +3354,37 @@
         <x:f t="shared" si="1"/>
         <x:v>45473</x:v>
       </x:c>
-      <x:c r="B34" s="35">
+      <x:c r="B34" s="19">
         <x:f t="shared" si="0"/>
         <x:v>45473</x:v>
       </x:c>
       <x:c r="C34" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D34" s="6"/>
       <x:c r="E34" s="6"/>
       <x:c r="F34" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="G34" s="6"/>
       <x:c r="H34" s="6"/>
       <x:c r="I34" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="J34" s="6"/>
       <x:c r="K34" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L34" s="6"/>
       <x:c r="M34" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:13">
       <x:c r="A35" s="4" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="B35" s="35"/>
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B35" s="19"/>
       <x:c r="C35" s="2">
         <x:f>COUNTA(C4:C34)</x:f>
         <x:v>12</x:v>
@@ -3451,36 +3477,36 @@
   </x:cols>
   <x:sheetData>
     <x:row r="7" spans="2:10">
-      <x:c r="B7" s="22" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="C7" s="23"/>
-      <x:c r="D7" s="23"/>
-      <x:c r="E7" s="22" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="F7" s="23"/>
-      <x:c r="G7" s="26"/>
-      <x:c r="H7" s="23" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="I7" s="23"/>
-      <x:c r="J7" s="26"/>
+      <x:c r="B7" s="26" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C7" s="27"/>
+      <x:c r="D7" s="27"/>
+      <x:c r="E7" s="26" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="F7" s="27"/>
+      <x:c r="G7" s="30"/>
+      <x:c r="H7" s="27" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="I7" s="27"/>
+      <x:c r="J7" s="30"/>
     </x:row>
     <x:row r="8" spans="2:10">
-      <x:c r="B8" s="24"/>
-      <x:c r="C8" s="25"/>
-      <x:c r="D8" s="25"/>
-      <x:c r="E8" s="24"/>
-      <x:c r="F8" s="25"/>
-      <x:c r="G8" s="27"/>
-      <x:c r="H8" s="25"/>
-      <x:c r="I8" s="25"/>
-      <x:c r="J8" s="27"/>
+      <x:c r="B8" s="28"/>
+      <x:c r="C8" s="29"/>
+      <x:c r="D8" s="29"/>
+      <x:c r="E8" s="28"/>
+      <x:c r="F8" s="29"/>
+      <x:c r="G8" s="31"/>
+      <x:c r="H8" s="29"/>
+      <x:c r="I8" s="29"/>
+      <x:c r="J8" s="31"/>
     </x:row>
     <x:row r="9" spans="2:10">
       <x:c r="B9" s="9" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C9" s="7">
         <x:v>3</x:v>
@@ -3489,7 +3515,7 @@
         <x:v>126000</x:v>
       </x:c>
       <x:c r="E9" s="9" t="s">
-        <x:v>29</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="F9" s="7">
         <x:v>2</x:v>
@@ -3499,7 +3525,7 @@
         <x:v>4000</x:v>
       </x:c>
       <x:c r="H9" s="7" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="I9" s="7">
         <x:v>7</x:v>
@@ -3510,7 +3536,7 @@
     </x:row>
     <x:row r="10" spans="2:10">
       <x:c r="B10" s="9" t="s">
-        <x:v>21</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C10" s="7">
         <x:v>1</x:v>
@@ -3521,7 +3547,7 @@
       <x:c r="E10" s="9"/>
       <x:c r="G10" s="10"/>
       <x:c r="H10" s="7" t="s">
-        <x:v>11</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="I10" s="7">
         <x:v>13</x:v>
@@ -3532,7 +3558,7 @@
     </x:row>
     <x:row r="11" spans="2:10">
       <x:c r="B11" s="9" t="s">
-        <x:v>18</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C11" s="7">
         <x:v>6</x:v>
@@ -3543,7 +3569,7 @@
       <x:c r="E11" s="9"/>
       <x:c r="G11" s="11"/>
       <x:c r="H11" s="7" t="s">
-        <x:v>29</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="I11" s="7">
         <x:v>4</x:v>
@@ -3572,15 +3598,15 @@
     <x:row r="13" spans="2:10">
       <x:c r="B13" s="9"/>
       <x:c r="C13" s="7" t="s">
-        <x:v>5</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E13" s="9"/>
       <x:c r="F13" s="7" t="s">
-        <x:v>7</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="G13" s="11"/>
       <x:c r="I13" s="7" t="s">
-        <x:v>6</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="J13" s="11"/>
     </x:row>
@@ -3609,11 +3635,11 @@
       <x:c r="J15" s="11"/>
     </x:row>
     <x:row r="16" spans="2:10" ht="13.949999999999999">
-      <x:c r="B16" s="28" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="C16" s="29"/>
-      <x:c r="D16" s="29"/>
+      <x:c r="B16" s="32" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C16" s="33"/>
+      <x:c r="D16" s="33"/>
       <x:c r="E16" s="14">
         <x:f>C14+F14</x:f>
         <x:v>16800</x:v>
@@ -3622,11 +3648,11 @@
       <x:c r="J16" s="11"/>
     </x:row>
     <x:row r="17" spans="2:10" ht="13.949999999999999" customHeight="1">
-      <x:c r="B17" s="30" t="s">
+      <x:c r="B17" s="34" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="C17" s="31"/>
-      <x:c r="D17" s="31"/>
+      <x:c r="C17" s="35"/>
+      <x:c r="D17" s="35"/>
       <x:c r="E17" s="15">
         <x:f>C14+I14</x:f>
         <x:v>26675</x:v>

</xml_diff>